<commit_message>
Updated partners and exchanged environment for place
</commit_message>
<xml_diff>
--- a/SFWS Action Plan.xlsx
+++ b/SFWS Action Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="267">
   <si>
     <t>S/M/L</t>
   </si>
@@ -154,12 +154,6 @@
     <t>Fewer young parents smoking at time of delivery</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Arun Wellbeing</t>
-  </si>
-  <si>
     <t>Pilot project 'Actively Quitting' using physical activity as a diversion</t>
   </si>
   <si>
@@ -223,9 +217,6 @@
     <t>Greater sharing of intelligence to Trading Standards</t>
   </si>
   <si>
-    <t>C/E</t>
-  </si>
-  <si>
     <t>More traders brought into  compliance, increase in numbes of seizures and quantities seized</t>
   </si>
   <si>
@@ -241,18 +232,12 @@
     <t>Reduction in 'hit rates' of sales in UAS operations</t>
   </si>
   <si>
-    <t>I/C/E</t>
-  </si>
-  <si>
     <t>Educate businesses in West Sussex in under age sales legislation</t>
   </si>
   <si>
     <t>Increased number of businesses with knowledge of UAS legislation and engagment with TS</t>
   </si>
   <si>
-    <t>Worthing Wellbeing</t>
-  </si>
-  <si>
     <t>Increase in the number of smokers acessing SSS from workplaces deprived areas</t>
   </si>
   <si>
@@ -268,9 +253,6 @@
     <t>A partnership that actively discusses and addresses through working together the tobacco issues in West Sussex</t>
   </si>
   <si>
-    <t xml:space="preserve"> E</t>
-  </si>
-  <si>
     <t>Effective stop smoking services reaching those that most need to access them</t>
   </si>
   <si>
@@ -433,9 +415,6 @@
     <t>Improve data capturing from stop smoking services</t>
   </si>
   <si>
-    <t>improve quality of stop smoking service delivery</t>
-  </si>
-  <si>
     <t>Develop a Patient Group Directive around Champix prescribing</t>
   </si>
   <si>
@@ -460,9 +439,6 @@
     <t>Report on the number of people signposted to stop smoking services from wellbeing hubs</t>
   </si>
   <si>
-    <t>Worthing Wellbeing, all hubs</t>
-  </si>
-  <si>
     <t>Referring young people who use Health4Families who are smokers to stop smoking services</t>
   </si>
   <si>
@@ -517,15 +493,9 @@
     <t>Western Sussex Hospitals NHS Foundation Trust</t>
   </si>
   <si>
-    <t>Arun Wellbeing, Health4Families, Trading Standards, Worthing Wellbeing</t>
-  </si>
-  <si>
     <t>Develop the role of the wellbeing programme to support tobacco control</t>
   </si>
   <si>
-    <t>Maternity at Western Hospitals, Arun Wellbeing, Health4Families, Worthing Wellbeing</t>
-  </si>
-  <si>
     <t>ap_number</t>
   </si>
   <si>
@@ -703,9 +673,6 @@
     <t>partners</t>
   </si>
   <si>
-    <t>All hubs</t>
-  </si>
-  <si>
     <t>level</t>
   </si>
   <si>
@@ -821,6 +788,36 @@
   </si>
   <si>
     <t>Explore how planning and licensing processes in local authorities can be utilised to promote  smokefree environments</t>
+  </si>
+  <si>
+    <t>Wellbeing programme</t>
+  </si>
+  <si>
+    <t>Maternity at Western Hospitals, Wellbeing programme, Health4Families</t>
+  </si>
+  <si>
+    <t>C/P</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P</t>
+  </si>
+  <si>
+    <t>I/C/P</t>
+  </si>
+  <si>
+    <t>Public Health, District &amp; Boroughs</t>
+  </si>
+  <si>
+    <t>Public Health, Primary Care</t>
+  </si>
+  <si>
+    <t>Wellbeing programme, Health4Families, Trading Standards, District &amp; Boroughs, Public Health</t>
+  </si>
+  <si>
+    <t>Improve quality of stop smoking service delivery</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,40 +1204,40 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>1</v>
@@ -1251,16 +1248,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1286,16 +1283,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1321,10 +1318,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>16</v>
@@ -1356,16 +1353,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1382,7 +1379,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>68</v>
+        <v>259</v>
       </c>
       <c r="M5" s="3"/>
     </row>
@@ -1391,16 +1388,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1426,16 +1423,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1461,16 +1458,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1496,16 +1493,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1531,16 +1528,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1601,16 +1598,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1630,7 +1627,7 @@
         <v>20</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1638,16 +1635,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1655,16 +1652,16 @@
         <v>3</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="M13" s="3"/>
     </row>
@@ -1673,16 +1670,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1690,10 +1687,10 @@
         <v>3</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>10</v>
@@ -1708,16 +1705,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1725,10 +1722,10 @@
         <v>3</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>12</v>
@@ -1743,16 +1740,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1760,10 +1757,10 @@
         <v>3</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>10</v>
@@ -1778,16 +1775,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>77</v>
+        <v>257</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1795,10 +1792,10 @@
         <v>3</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>18</v>
@@ -1813,16 +1810,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1830,10 +1827,10 @@
         <v>3</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>10</v>
@@ -1848,16 +1845,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1865,10 +1862,10 @@
         <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>4</v>
@@ -1883,16 +1880,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1900,10 +1897,10 @@
         <v>3</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>10</v>
@@ -1918,16 +1915,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>166</v>
+        <v>265</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1953,7 +1950,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>17</v>
@@ -1988,16 +1985,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -2023,16 +2020,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -2049,7 +2046,7 @@
         <v>4</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="M24" s="3"/>
     </row>
@@ -2058,16 +2055,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -2093,13 +2090,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>2</v>
@@ -2128,16 +2125,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -2163,16 +2160,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2198,16 +2195,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2233,16 +2230,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -2268,16 +2265,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -2303,16 +2300,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>138</v>
+        <v>266</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>138</v>
+        <v>266</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -2338,16 +2335,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -2373,7 +2370,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>33</v>
@@ -2408,16 +2405,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -2443,16 +2440,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2478,16 +2475,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -2513,16 +2510,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -2548,16 +2545,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -2583,10 +2580,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -2618,10 +2615,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>11</v>
@@ -2653,16 +2650,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -2688,10 +2685,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>23</v>
@@ -2723,16 +2720,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -2758,16 +2755,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2793,16 +2790,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2828,16 +2825,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2863,10 +2860,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>6</v>
@@ -2898,16 +2895,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2927,7 +2924,7 @@
         <v>5</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2935,16 +2932,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -2970,16 +2967,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -3005,10 +3002,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>24</v>
@@ -3040,10 +3037,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>13</v>
@@ -3075,16 +3072,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -3101,10 +3098,10 @@
         <v>0</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>68</v>
+        <v>259</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3112,16 +3109,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -3138,10 +3135,10 @@
         <v>0</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>68</v>
+        <v>259</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3152,13 +3149,13 @@
         <v>37</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>168</v>
+        <v>258</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -3184,16 +3181,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -3201,16 +3198,16 @@
         <v>8</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K57" s="3" t="s">
         <v>4</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>83</v>
+        <v>261</v>
       </c>
       <c r="M57" s="3"/>
     </row>
@@ -3219,16 +3216,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -3236,16 +3233,16 @@
         <v>8</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="M58" s="3"/>
     </row>
@@ -3254,16 +3251,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -3271,10 +3268,10 @@
         <v>8</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>4</v>
@@ -3289,16 +3286,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -3306,10 +3303,10 @@
         <v>8</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>4</v>
@@ -3324,16 +3321,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -3341,16 +3338,16 @@
         <v>8</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K61" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="M61" s="3"/>
     </row>
@@ -3359,16 +3356,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -3385,10 +3382,10 @@
         <v>0</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>74</v>
+        <v>262</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3396,16 +3393,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -3422,10 +3419,10 @@
         <v>0</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>74</v>
+        <v>262</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3433,16 +3430,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -3468,16 +3465,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -3503,16 +3500,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -3538,7 +3535,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>41</v>
@@ -3573,16 +3570,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -3608,16 +3605,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -3641,10 +3638,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>27</v>
@@ -3676,16 +3673,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -3711,16 +3708,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -3737,10 +3734,10 @@
         <v>4</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3748,13 +3745,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>21</v>
@@ -3774,7 +3771,7 @@
         <v>10</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="M73" s="3"/>
     </row>
@@ -3783,16 +3780,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="H74" s="3">
         <v>10</v>
@@ -3807,7 +3804,7 @@
         <v>10</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>45</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Wellbeing Programme actions and MECC primary care
</commit_message>
<xml_diff>
--- a/SFWS Action Plan.xlsx
+++ b/SFWS Action Plan.xlsx
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,7 +2834,7 @@
         <v>93</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>74</v>
+        <v>264</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3820,26 +3820,10 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f0a195-02ac-4a72-b655-6664c0f36d60" ContentTypeId="0x01010008FB9B3217D433459C91B5CF793C1D79" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CSMeta2010Field xmlns="http://schemas.microsoft.com/sharepoint/v3">6001052b-8a4f-49a5-9104-ed2894940f4d;2019-01-23 09:46:40;PENDINGCLASSIFICATION;WSCC Category:|False||PENDINGCLASSIFICATION|2019-01-23 09:46:40|UNDEFINED|35da7913-ca98-450a-b299-b9b62231058f;False</CSMeta2010Field>
-    <j5da7913ca98450ab299b9b62231058f xmlns="1209568c-8f7e-4a25-939e-4f22fd0c2b25">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j5da7913ca98450ab299b9b62231058f>
-    <TaxCatchAll xmlns="1209568c-8f7e-4a25-939e-4f22fd0c2b25"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="WSCC Document" ma:contentTypeID="0x01010008FB9B3217D433459C91B5CF793C1D79007461669338EA85489E4BA6CA2B3BA852" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="ae4bde9a2964b34326abd15481a333b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1209568c-8f7e-4a25-939e-4f22fd0c2b25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f04673fdb785c505355dc3028254dfa8" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4002,9 +3986,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CSMeta2010Field xmlns="http://schemas.microsoft.com/sharepoint/v3">6001052b-8a4f-49a5-9104-ed2894940f4d;2019-01-23 09:46:40;PENDINGCLASSIFICATION;WSCC Category:|False||PENDINGCLASSIFICATION|2019-01-23 09:46:40|UNDEFINED|35da7913-ca98-450a-b299-b9b62231058f;False</CSMeta2010Field>
+    <j5da7913ca98450ab299b9b62231058f xmlns="1209568c-8f7e-4a25-939e-4f22fd0c2b25">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j5da7913ca98450ab299b9b62231058f>
+    <TaxCatchAll xmlns="1209568c-8f7e-4a25-939e-4f22fd0c2b25"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f0a195-02ac-4a72-b655-6664c0f36d60" ContentTypeId="0x01010008FB9B3217D433459C91B5CF793C1D79" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4074,31 +4074,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90D2BF52-903F-47A7-9E65-A1ECE2CB776A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7EF8C93-57EF-45EC-BAE9-9308FAEFD416}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81DA5304-C145-49A6-B089-CBFEBCB5A12C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="1209568c-8f7e-4a25-939e-4f22fd0c2b25"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C49D17-E123-4DE8-9436-DC182C7BC6DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4117,10 +4100,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81DA5304-C145-49A6-B089-CBFEBCB5A12C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1209568c-8f7e-4a25-939e-4f22fd0c2b25"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7EF8C93-57EF-45EC-BAE9-9308FAEFD416}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90D2BF52-903F-47A7-9E65-A1ECE2CB776A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>